<commit_message>
RegistrationPage , Test and properties
</commit_message>
<xml_diff>
--- a/FinalProject/data/pet-store-data.xlsx
+++ b/FinalProject/data/pet-store-data.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21225" windowHeight="7185" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="cart_items" sheetId="1" r:id="rId1"/>
     <sheet name="users" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:H13"/>
 </workbook>
 </file>
 
@@ -1415,8 +1416,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1583,6 +1584,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1629,7 +1638,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1661,9 +1670,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1695,6 +1705,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1870,20 +1881,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.140625" customWidth="1"/>
     <col min="2" max="2" width="108" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1891,7 +1902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>445</v>
       </c>
@@ -1899,7 +1910,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>447</v>
       </c>
@@ -1907,7 +1918,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>449</v>
       </c>
@@ -1915,7 +1926,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>452</v>
       </c>
@@ -1923,7 +1934,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>454</v>
       </c>
@@ -1931,7 +1942,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>455</v>
       </c>
@@ -1939,7 +1950,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>458</v>
       </c>
@@ -1947,7 +1958,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>460</v>
       </c>
@@ -1955,7 +1966,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>462</v>
       </c>
@@ -1963,7 +1974,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>463</v>
       </c>
@@ -1989,14 +2000,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="4" width="17.28515625" style="3"/>
     <col min="5" max="5" width="25.85546875" style="3" customWidth="1"/>
@@ -2005,7 +2016,7 @@
     <col min="8" max="16384" width="17.28515625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="30.75" thickBot="1">
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2043,7 +2054,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="44.25" thickBot="1">
+    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -2081,7 +2092,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="44.25" thickBot="1">
+    <row r="3" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -2119,7 +2130,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="58.5" thickBot="1">
+    <row r="4" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -2157,7 +2168,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="58.5" thickBot="1">
+    <row r="5" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -2195,7 +2206,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="44.25" thickBot="1">
+    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -2233,7 +2244,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="44.25" thickBot="1">
+    <row r="7" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -2271,7 +2282,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="44.25" thickBot="1">
+    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -2309,7 +2320,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="44.25" thickBot="1">
+    <row r="9" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -2347,7 +2358,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="58.5" thickBot="1">
+    <row r="10" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>9</v>
       </c>
@@ -2385,7 +2396,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="58.5" thickBot="1">
+    <row r="11" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -2423,7 +2434,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="58.5" thickBot="1">
+    <row r="12" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -2461,7 +2472,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="44.25" thickBot="1">
+    <row r="13" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
         <v>12</v>
       </c>
@@ -2499,7 +2510,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="44.25" thickBot="1">
+    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -2537,7 +2548,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="44.25" thickBot="1">
+    <row r="15" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -2575,7 +2586,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="44.25" thickBot="1">
+    <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
         <v>15</v>
       </c>
@@ -2613,7 +2624,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="44.25" thickBot="1">
+    <row r="17" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -2651,7 +2662,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="44.25" thickBot="1">
+    <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -2689,7 +2700,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="44.25" thickBot="1">
+    <row r="19" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7">
         <v>18</v>
       </c>
@@ -2727,7 +2738,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="44.25" thickBot="1">
+    <row r="20" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -2765,7 +2776,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="44.25" thickBot="1">
+    <row r="21" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -2803,7 +2814,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="44.25" thickBot="1">
+    <row r="22" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7">
         <v>21</v>
       </c>
@@ -2841,7 +2852,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="58.5" thickBot="1">
+    <row r="23" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -2879,7 +2890,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="44.25" thickBot="1">
+    <row r="24" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -2917,7 +2928,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="58.5" thickBot="1">
+    <row r="25" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7">
         <v>24</v>
       </c>
@@ -2955,7 +2966,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="58.5" thickBot="1">
+    <row r="26" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>25</v>
       </c>
@@ -2993,7 +3004,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="58.5" thickBot="1">
+    <row r="27" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>26</v>
       </c>
@@ -3031,7 +3042,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="44.25" thickBot="1">
+    <row r="28" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="7">
         <v>27</v>
       </c>
@@ -3069,7 +3080,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="58.5" thickBot="1">
+    <row r="29" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>28</v>
       </c>
@@ -3107,7 +3118,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="44.25" thickBot="1">
+    <row r="30" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>29</v>
       </c>
@@ -3145,7 +3156,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="58.5" thickBot="1">
+    <row r="31" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="7">
         <v>30</v>
       </c>
@@ -3183,7 +3194,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="44.25" thickBot="1">
+    <row r="32" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -3221,7 +3232,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="58.5" thickBot="1">
+    <row r="33" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -3259,7 +3270,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="44.25" thickBot="1">
+    <row r="34" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="7">
         <v>33</v>
       </c>
@@ -3297,7 +3308,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="58.5" thickBot="1">
+    <row r="35" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>34</v>
       </c>
@@ -3335,7 +3346,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="58.5" thickBot="1">
+    <row r="36" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>35</v>
       </c>
@@ -3373,7 +3384,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="44.25" thickBot="1">
+    <row r="37" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="7">
         <v>36</v>
       </c>
@@ -3411,7 +3422,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="44.25" thickBot="1">
+    <row r="38" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>37</v>
       </c>
@@ -3449,7 +3460,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="58.5" thickBot="1">
+    <row r="39" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>38</v>
       </c>
@@ -3487,7 +3498,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="44.25" thickBot="1">
+    <row r="40" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="7">
         <v>39</v>
       </c>
@@ -3525,7 +3536,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="44.25" thickBot="1">
+    <row r="41" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>40</v>
       </c>
@@ -3563,7 +3574,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="58.5" thickBot="1">
+    <row r="42" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
         <v>41</v>
       </c>
@@ -3601,7 +3612,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="44.25" thickBot="1">
+    <row r="43" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="7">
         <v>42</v>
       </c>
@@ -3639,7 +3650,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="58.5" thickBot="1">
+    <row r="44" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
         <v>43</v>
       </c>
@@ -3677,7 +3688,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="58.5" thickBot="1">
+    <row r="45" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <v>44</v>
       </c>
@@ -3715,7 +3726,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="44.25" thickBot="1">
+    <row r="46" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="7">
         <v>45</v>
       </c>
@@ -3753,7 +3764,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="58.5" thickBot="1">
+    <row r="47" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
         <v>46</v>
       </c>
@@ -3791,7 +3802,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="44.25" thickBot="1">
+    <row r="48" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <v>47</v>
       </c>
@@ -3829,7 +3840,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="44.25" thickBot="1">
+    <row r="49" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="7">
         <v>48</v>
       </c>
@@ -3867,7 +3878,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="44.25" thickBot="1">
+    <row r="50" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4">
         <v>49</v>
       </c>
@@ -3905,7 +3916,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="44.25" thickBot="1">
+    <row r="51" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4">
         <v>50</v>
       </c>

</xml_diff>

<commit_message>
SiginPage/Test and RegistrationPage fix
</commit_message>
<xml_diff>
--- a/FinalProject/data/pet-store-data.xlsx
+++ b/FinalProject/data/pet-store-data.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21225" windowHeight="7185" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="cart_items" sheetId="1" r:id="rId1"/>
     <sheet name="users" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1:J13"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -1416,8 +1415,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1584,14 +1583,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1638,7 +1629,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1670,10 +1661,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1705,7 +1695,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1881,20 +1870,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28.140625" customWidth="1"/>
     <col min="2" max="2" width="108" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1902,7 +1891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="12" t="s">
         <v>445</v>
       </c>
@@ -1910,7 +1899,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="12" t="s">
         <v>447</v>
       </c>
@@ -1918,7 +1907,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="12" t="s">
         <v>449</v>
       </c>
@@ -1926,7 +1915,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="12" t="s">
         <v>452</v>
       </c>
@@ -1934,7 +1923,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="12" t="s">
         <v>454</v>
       </c>
@@ -1942,7 +1931,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" s="12" t="s">
         <v>455</v>
       </c>
@@ -1950,7 +1939,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" s="12" t="s">
         <v>458</v>
       </c>
@@ -1958,7 +1947,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" s="12" t="s">
         <v>460</v>
       </c>
@@ -1966,7 +1955,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10" s="12" t="s">
         <v>462</v>
       </c>
@@ -1974,7 +1963,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" s="12" t="s">
         <v>463</v>
       </c>
@@ -2000,14 +1989,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="4" width="17.28515625" style="3"/>
     <col min="5" max="5" width="25.85546875" style="3" customWidth="1"/>
@@ -2016,7 +2005,7 @@
     <col min="8" max="16384" width="17.28515625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="30.75" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2054,7 +2043,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="44.25" thickBot="1">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -2092,7 +2081,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="44.25" thickBot="1">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -2130,7 +2119,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="58.5" thickBot="1">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -2168,7 +2157,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="58.5" thickBot="1">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -2206,7 +2195,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="44.25" thickBot="1">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -2244,7 +2233,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="44.25" thickBot="1">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -2282,7 +2271,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="44.25" thickBot="1">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -2320,7 +2309,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="44.25" thickBot="1">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -2358,7 +2347,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="58.5" thickBot="1">
       <c r="A10" s="7">
         <v>9</v>
       </c>
@@ -2396,7 +2385,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="58.5" thickBot="1">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -2434,7 +2423,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="58.5" thickBot="1">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -2472,7 +2461,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="44.25" thickBot="1">
       <c r="A13" s="7">
         <v>12</v>
       </c>
@@ -2510,7 +2499,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="44.25" thickBot="1">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -2548,7 +2537,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="44.25" thickBot="1">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -2586,7 +2575,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="44.25" thickBot="1">
       <c r="A16" s="7">
         <v>15</v>
       </c>
@@ -2624,7 +2613,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="44.25" thickBot="1">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -2662,7 +2651,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="44.25" thickBot="1">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -2700,7 +2689,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="44.25" thickBot="1">
       <c r="A19" s="7">
         <v>18</v>
       </c>
@@ -2738,7 +2727,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="44.25" thickBot="1">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -2776,7 +2765,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="44.25" thickBot="1">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -2814,7 +2803,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" ht="44.25" thickBot="1">
       <c r="A22" s="7">
         <v>21</v>
       </c>
@@ -2852,7 +2841,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" ht="58.5" thickBot="1">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -2890,7 +2879,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" ht="44.25" thickBot="1">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -2928,7 +2917,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" ht="58.5" thickBot="1">
       <c r="A25" s="7">
         <v>24</v>
       </c>
@@ -2966,7 +2955,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" ht="58.5" thickBot="1">
       <c r="A26" s="4">
         <v>25</v>
       </c>
@@ -3004,7 +2993,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" ht="58.5" thickBot="1">
       <c r="A27" s="4">
         <v>26</v>
       </c>
@@ -3042,7 +3031,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" ht="44.25" thickBot="1">
       <c r="A28" s="7">
         <v>27</v>
       </c>
@@ -3080,7 +3069,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" ht="58.5" thickBot="1">
       <c r="A29" s="4">
         <v>28</v>
       </c>
@@ -3118,7 +3107,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" ht="44.25" thickBot="1">
       <c r="A30" s="4">
         <v>29</v>
       </c>
@@ -3156,7 +3145,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" ht="58.5" thickBot="1">
       <c r="A31" s="7">
         <v>30</v>
       </c>
@@ -3194,7 +3183,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" ht="44.25" thickBot="1">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -3232,7 +3221,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" ht="58.5" thickBot="1">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -3270,7 +3259,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" ht="44.25" thickBot="1">
       <c r="A34" s="7">
         <v>33</v>
       </c>
@@ -3308,7 +3297,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" ht="58.5" thickBot="1">
       <c r="A35" s="4">
         <v>34</v>
       </c>
@@ -3346,7 +3335,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" ht="58.5" thickBot="1">
       <c r="A36" s="4">
         <v>35</v>
       </c>
@@ -3384,7 +3373,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" ht="44.25" thickBot="1">
       <c r="A37" s="7">
         <v>36</v>
       </c>
@@ -3422,7 +3411,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" ht="44.25" thickBot="1">
       <c r="A38" s="4">
         <v>37</v>
       </c>
@@ -3460,7 +3449,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" ht="58.5" thickBot="1">
       <c r="A39" s="4">
         <v>38</v>
       </c>
@@ -3498,7 +3487,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" ht="44.25" thickBot="1">
       <c r="A40" s="7">
         <v>39</v>
       </c>
@@ -3536,7 +3525,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" ht="44.25" thickBot="1">
       <c r="A41" s="4">
         <v>40</v>
       </c>
@@ -3574,7 +3563,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" ht="58.5" thickBot="1">
       <c r="A42" s="4">
         <v>41</v>
       </c>
@@ -3612,7 +3601,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" ht="44.25" thickBot="1">
       <c r="A43" s="7">
         <v>42</v>
       </c>
@@ -3650,7 +3639,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" ht="58.5" thickBot="1">
       <c r="A44" s="4">
         <v>43</v>
       </c>
@@ -3688,7 +3677,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" ht="58.5" thickBot="1">
       <c r="A45" s="4">
         <v>44</v>
       </c>
@@ -3726,7 +3715,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" ht="44.25" thickBot="1">
       <c r="A46" s="7">
         <v>45</v>
       </c>
@@ -3764,7 +3753,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" ht="58.5" thickBot="1">
       <c r="A47" s="4">
         <v>46</v>
       </c>
@@ -3802,7 +3791,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" ht="44.25" thickBot="1">
       <c r="A48" s="4">
         <v>47</v>
       </c>
@@ -3840,7 +3829,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" ht="44.25" thickBot="1">
       <c r="A49" s="7">
         <v>48</v>
       </c>
@@ -3878,7 +3867,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" ht="44.25" thickBot="1">
       <c r="A50" s="4">
         <v>49</v>
       </c>
@@ -3916,7 +3905,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" ht="44.25" thickBot="1">
       <c r="A51" s="4">
         <v>50</v>
       </c>

</xml_diff>

<commit_message>
RegistrationPage/Test and pet-store-data commit
</commit_message>
<xml_diff>
--- a/FinalProject/data/pet-store-data.xlsx
+++ b/FinalProject/data/pet-store-data.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="cart_items" sheetId="1" r:id="rId1"/>
     <sheet name="users" sheetId="2" r:id="rId2"/>
+    <sheet name="users_without_password" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <oleSize ref="A1:H20"/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="515">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="565">
   <si>
     <t>ITEM_ID</t>
   </si>
@@ -1413,154 +1414,304 @@
     <t>https://petstore.octoperf.com/actions/Catalog.action?viewItem=&amp;itemId=EST-13</t>
   </si>
   <si>
-    <t>vetrPHh7r5XnwwA16bHH1</t>
-  </si>
-  <si>
-    <t>nBzzSHIeWHtL3Ny9Y3b6u</t>
-  </si>
-  <si>
-    <t>uTIHfVfhh56umnkAzRMtE</t>
-  </si>
-  <si>
-    <t>bxEyqN9f571BzGFLqVgyJ</t>
-  </si>
-  <si>
-    <t>guwLgx6eGYMbCK4mCcB8B</t>
-  </si>
-  <si>
-    <t>mTtDA175kNsnctWgOyQMq</t>
-  </si>
-  <si>
-    <t>VjeOGITROl5XnTG94CQD4</t>
-  </si>
-  <si>
-    <t>DDE3A0XNEEaaMc1GQGMVO</t>
-  </si>
-  <si>
-    <t>wyWgh0tj7GNHMglGMhtw_</t>
-  </si>
-  <si>
-    <t>bZqba0EhWau3161oPqcL9</t>
-  </si>
-  <si>
-    <t>4B9lzPH5LngCaOv2cmJ70</t>
-  </si>
-  <si>
-    <t>-Cg44ePS6y3ySr9tScp1a</t>
-  </si>
-  <si>
-    <t>PtQMVKqiS2AW2gAUMtS2u</t>
-  </si>
-  <si>
-    <t>PfWKY3-qig7o-5HTWWPkJ</t>
-  </si>
-  <si>
-    <t>ndos6sb58-sAgqUTkTQnX</t>
-  </si>
-  <si>
-    <t>2UubMcHL1agfhjeJkSB4Y</t>
-  </si>
-  <si>
-    <t>qYWcp1K09ZQBvoHRjnP91</t>
-  </si>
-  <si>
-    <t>u3VolF3BUkmDepQZ0RBtI</t>
-  </si>
-  <si>
-    <t>OFLfcsA2K0HJhtbJXVEnJ</t>
-  </si>
-  <si>
-    <t>Ar3RvsYxmPsMFGRI_01TX</t>
-  </si>
-  <si>
-    <t>6s21wAOq7gfK2i2nsQKUC</t>
-  </si>
-  <si>
-    <t>m1Z0caC2DLpgw51_4hbkh</t>
-  </si>
-  <si>
-    <t>WAQRoQdfwwSer0n-tCDtZ</t>
-  </si>
-  <si>
-    <t>S0TrVbBl91xP12SHEXr2Q</t>
-  </si>
-  <si>
-    <t>rmw8Hn66_6pzkVUt-AyqK</t>
-  </si>
-  <si>
-    <t>S5lKldNDv2EoObcrs7wo8</t>
-  </si>
-  <si>
-    <t>etTNQJNNnUEyXdxuG-hgt</t>
-  </si>
-  <si>
-    <t>pmqfetgiGSCGl8EhgfQBA</t>
-  </si>
-  <si>
-    <t>E0JP7hYmBDN_2N5zAPnov</t>
-  </si>
-  <si>
-    <t>MW_HVOPn_liTFizeyFPsK</t>
-  </si>
-  <si>
-    <t>6FK7B6aMuNkjftumBwtAJ</t>
-  </si>
-  <si>
-    <t>fAY7E-L7oGZnW_s8OIkEa</t>
-  </si>
-  <si>
-    <t>anhC3bSAtD6n3RSne9xdq</t>
-  </si>
-  <si>
-    <t>_iI4Ntq3Yz7qvK585J1wU</t>
-  </si>
-  <si>
-    <t>tEr2mAwAJB-aWTEAvfMN6</t>
-  </si>
-  <si>
-    <t>zdhLhPyhBD3Ox-x7T2Emx</t>
-  </si>
-  <si>
-    <t>TetdvDDiavVqI4d1ldnAu</t>
-  </si>
-  <si>
-    <t>zwK8oWHkuzWxbK_dQTE92</t>
-  </si>
-  <si>
-    <t>_cu4OIi6VAxNh8ROeBUC8</t>
-  </si>
-  <si>
-    <t>gdmS7m5uN8BKHAcy6eC-I</t>
-  </si>
-  <si>
-    <t>DirR8iBudnjofb_DO2-70</t>
-  </si>
-  <si>
-    <t>5tNfL-na9tHtoA9g-pfkC</t>
-  </si>
-  <si>
-    <t>ruaeM7PBUX7IyWrqjbiOH</t>
-  </si>
-  <si>
-    <t>8pVEdMMoGqVu-psVt92Xi</t>
-  </si>
-  <si>
-    <t>yZeksvxekiLE-EtVxLIP0</t>
-  </si>
-  <si>
-    <t>0ifjfTow9n7ADYGp28SeT</t>
-  </si>
-  <si>
-    <t>a-vn5NTHmlYue4JMz3Azt</t>
-  </si>
-  <si>
-    <t>IOClLTYdVp9ch5P5ITIrD</t>
-  </si>
-  <si>
-    <t>71hrUhcYLBDb7aPrW_pE2</t>
-  </si>
-  <si>
-    <t>2mggVpoALphXjZ2dL4RWW</t>
+    <t>ABbpPrZJgWLHecLjJl5dy</t>
+  </si>
+  <si>
+    <t>mnrR8JB_klTm8DZM5eTls</t>
+  </si>
+  <si>
+    <t>VxFjJMN-eI9Byvu3nZYZW</t>
+  </si>
+  <si>
+    <t>s32MkZ7vTlqeUz4URVHQE</t>
+  </si>
+  <si>
+    <t>rlZJ0S6ymM9wC66CbuoAh</t>
+  </si>
+  <si>
+    <t>YjbJFYZzc_dd1cobMiWu_</t>
+  </si>
+  <si>
+    <t>GvLSJj_WuROsX8Tnv0rEA</t>
+  </si>
+  <si>
+    <t>XftNPrpXSW0Qc_Mc1fmfe</t>
+  </si>
+  <si>
+    <t>VFNdKXfoa3P9XsGwpaXGP</t>
+  </si>
+  <si>
+    <t>ggJt4SlVDK-TUsTMjyb5K</t>
+  </si>
+  <si>
+    <t>ogiX32BJopnUFW4iw3j57</t>
+  </si>
+  <si>
+    <t>v4s6alZ_tMh4fq7MPufCV</t>
+  </si>
+  <si>
+    <t>5a4cbTAu30-C0QQtioxTV</t>
+  </si>
+  <si>
+    <t>-mia5tcLoEhe8JVCmrJiV</t>
+  </si>
+  <si>
+    <t>HFRnFi145Ak9D0Ue5XrbH</t>
+  </si>
+  <si>
+    <t>vs1-HYNusjhj62iRLjOQw</t>
+  </si>
+  <si>
+    <t>WraAVP6-O-w801i6c2HO1</t>
+  </si>
+  <si>
+    <t>XN7kiVCQWbKed76nBk7VH</t>
+  </si>
+  <si>
+    <t>EXI2L7zZbJr3ao57w7lQf</t>
+  </si>
+  <si>
+    <t>1bmisEZ0wifiGV2pNxexH</t>
+  </si>
+  <si>
+    <t>xZ0iVVcipbchwoqcA66WD</t>
+  </si>
+  <si>
+    <t>QuZdoi1k0Mi8xkFGHkun4</t>
+  </si>
+  <si>
+    <t>vLPfi5t4Y31o5NJP3YUzX</t>
+  </si>
+  <si>
+    <t>JlGhuUJlhNeWsNlQr5sX9</t>
+  </si>
+  <si>
+    <t>Vqe4D8gmvhPsFJ3q1ucFe</t>
+  </si>
+  <si>
+    <t>SkMzxT9_hxladNwW5s3cn</t>
+  </si>
+  <si>
+    <t>yXMM4LOU-UL4PUBQku5GY</t>
+  </si>
+  <si>
+    <t>zQ8KAFrq0cbSho2VXJVCp</t>
+  </si>
+  <si>
+    <t>EU3HT_I4rrgh_Yc5TjJyK</t>
+  </si>
+  <si>
+    <t>Br1AU8vbkd2ZVTK2LYHR_</t>
+  </si>
+  <si>
+    <t>1Ccle0PAD2qQM6hLmjQlD</t>
+  </si>
+  <si>
+    <t>RSSlXeY5cGICHkNEOa0gA</t>
+  </si>
+  <si>
+    <t>UfcHZqro2yPi72496hTaO</t>
+  </si>
+  <si>
+    <t>PPmAtOwjZRoFBNpGy-wuq</t>
+  </si>
+  <si>
+    <t>tOYiw-PvKQfE25nyIKJNP</t>
+  </si>
+  <si>
+    <t>TDTWVKfm--yRq65QVGvJ6</t>
+  </si>
+  <si>
+    <t>9EUJznKj-asTUtS_jDnMZ</t>
+  </si>
+  <si>
+    <t>5PRJfR8-nAPazZs9o8MaP</t>
+  </si>
+  <si>
+    <t>I8_0BD13TcOWAYk745JMs</t>
+  </si>
+  <si>
+    <t>ogOleczG-X4pt8NepM6AR</t>
+  </si>
+  <si>
+    <t>hLZhZdmR1ARqGXvkgFagg</t>
+  </si>
+  <si>
+    <t>jXbvII0IVe1WCHw5Hf-Wc</t>
+  </si>
+  <si>
+    <t>v9iuWQ3FaSgZ0XufCUGvC</t>
+  </si>
+  <si>
+    <t>ZYAY5CGix06gc6z6fT-wC</t>
+  </si>
+  <si>
+    <t>jwts_HfppIm4DJN-oWAeA</t>
+  </si>
+  <si>
+    <t>mF6pviiRrtkKF4e-wsqRh</t>
+  </si>
+  <si>
+    <t>TUd8fEwjuggbkYAj361xS</t>
+  </si>
+  <si>
+    <t>AnbaKNjMCCiNhivViWppO</t>
+  </si>
+  <si>
+    <t>vmpzk8TYITOSUzZj_xgyB</t>
+  </si>
+  <si>
+    <t>hrqn7qAinDQwBHuGQebAb</t>
+  </si>
+  <si>
+    <t>eH0IrLwD37oLQuIt9UZsH</t>
+  </si>
+  <si>
+    <t>eUmLcHrOxRF37jI1UAM1t</t>
+  </si>
+  <si>
+    <t>LotA1DbhYQSwvI1yqPU4L</t>
+  </si>
+  <si>
+    <t>B2KA_hiyIYAR9KzfhN0L4</t>
+  </si>
+  <si>
+    <t>ogmWyovezRITiXYwmFewx</t>
+  </si>
+  <si>
+    <t>5ZOWxhjG40iXsBHSlD65V</t>
+  </si>
+  <si>
+    <t>gJcu7zL1pxt8PYU2EU76M</t>
+  </si>
+  <si>
+    <t>lKUlBD72YkoBcIUv3VfRK</t>
+  </si>
+  <si>
+    <t>38RugvUNBydvTlmheTvT8</t>
+  </si>
+  <si>
+    <t>lI267LtIvkDsu3LtbVxU2</t>
+  </si>
+  <si>
+    <t>qd90bl1vNijZIzy-T6Tkk</t>
+  </si>
+  <si>
+    <t>fbplhm552lpsDoos-F81d</t>
+  </si>
+  <si>
+    <t>JCgt3RANHC_Ts3aTahySI</t>
+  </si>
+  <si>
+    <t>zWuiekBlFTATKJohoR_WD</t>
+  </si>
+  <si>
+    <t>9pLrqfmwvuCFSxgQ1R2L5</t>
+  </si>
+  <si>
+    <t>Pk3XcezcGRdtu7VIk0VUD</t>
+  </si>
+  <si>
+    <t>hsLToIR1JY-vxIrppZWKf</t>
+  </si>
+  <si>
+    <t>_nhcqYWbrEc6X3nbICmmA</t>
+  </si>
+  <si>
+    <t>doWtq9K9BSNlCBobFGLtH</t>
+  </si>
+  <si>
+    <t>fh92EbG9WN6F90eyRhHAw</t>
+  </si>
+  <si>
+    <t>tJ3lvCHnBNqPt3QSCqOuP</t>
+  </si>
+  <si>
+    <t>j4C2oI8ZF9BOTabkvmOiH</t>
+  </si>
+  <si>
+    <t>R9UfX3cffu82RwM-6o0Mh</t>
+  </si>
+  <si>
+    <t>Pg1YOFuFdr9neiafFVgmv</t>
+  </si>
+  <si>
+    <t>NYgxewKag8ZaeBljrD0Py</t>
+  </si>
+  <si>
+    <t>DdJpCwHRuNRQvduc2PG7v</t>
+  </si>
+  <si>
+    <t>v3to55rnqkCut6kD27sCK</t>
+  </si>
+  <si>
+    <t>5nbWXy-Rls4fC5-4vpC3u</t>
+  </si>
+  <si>
+    <t>lVXduHpSclHoEl81NzG1Y</t>
+  </si>
+  <si>
+    <t>l_N7U1Z3DJCQdPVdZ-2rK</t>
+  </si>
+  <si>
+    <t>HiB8pPMk0FV3OwSqgdw8r</t>
+  </si>
+  <si>
+    <t>RYY0WUjxcKs85ZRLR2xQk</t>
+  </si>
+  <si>
+    <t>gUommyV3l5qmLWgJFMj_t</t>
+  </si>
+  <si>
+    <t>GV8Uv9cK43JDpVApUT-Mt</t>
+  </si>
+  <si>
+    <t>-ONfkNqgUktCDACHGOOzB</t>
+  </si>
+  <si>
+    <t>9R9CR_Y2YhjwfYSwfifYp</t>
+  </si>
+  <si>
+    <t>bQphyd-yBvpxPx5shyAA_</t>
+  </si>
+  <si>
+    <t>5CL0vUAHd2ZkyM4bhfSLY</t>
+  </si>
+  <si>
+    <t>quYtV0J3lLarex2meO-Ic</t>
+  </si>
+  <si>
+    <t>2vybb9QpBjKwMFIU7myhq</t>
+  </si>
+  <si>
+    <t>tcfZV3CjHo-_mjbMBDslw</t>
+  </si>
+  <si>
+    <t>r6zIYSEhK2sUDS9tcMSec</t>
+  </si>
+  <si>
+    <t>MyJyK1MWSXVJZz6tgNLMf</t>
+  </si>
+  <si>
+    <t>HP-HVAXLT-7PJs5UIIUWc</t>
+  </si>
+  <si>
+    <t>SOp3CKHqNFm5HKlTJMPAO</t>
+  </si>
+  <si>
+    <t>EpVs80DYUki6wPoGk0kF4</t>
+  </si>
+  <si>
+    <t>pwyEbcbN6_gy11uhgz8uF</t>
+  </si>
+  <si>
+    <t>xa2ciMjPr7IkoC6lHxmoF</t>
+  </si>
+  <si>
+    <t>7IMjkSglqHmXrKHwRdu3O</t>
+  </si>
+  <si>
+    <t>ImWUAe6XeCtnEhCyNbfoF</t>
   </si>
 </sst>
 </file>
@@ -2206,6 +2357,1967 @@
     </row>
     <row r="2" spans="1:12" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
+        <v>515</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="9">
+        <v>33101</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>516</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="9">
+        <v>23308</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>517</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="K4" s="9">
+        <v>26739</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>518</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="K5" s="9">
+        <v>74468</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>519</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="K6" s="9">
+        <v>28160</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>520</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="K7" s="9">
+        <v>15545</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>521</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="K8" s="9">
+        <v>65080</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>522</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="K9" s="9">
+        <v>82718</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>523</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="K10" s="9">
+        <v>10273</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>524</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="K11" s="9">
+        <v>58651</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>525</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="K12" s="9">
+        <v>46851</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>526</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="K13" s="9">
+        <v>15601</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>527</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K14" s="9">
+        <v>47992</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>528</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="K15" s="9">
+        <v>78338</v>
+      </c>
+      <c r="L15" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>529</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="K16" s="9">
+        <v>76465</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>530</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="K17" s="9">
+        <v>38369</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>531</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="K18" s="9">
+        <v>18449</v>
+      </c>
+      <c r="L18" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>532</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="K19" s="9">
+        <v>52640</v>
+      </c>
+      <c r="L19" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>533</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="J20" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="K20" s="9">
+        <v>15250</v>
+      </c>
+      <c r="L20" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>534</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="K21" s="9">
+        <v>93718</v>
+      </c>
+      <c r="L21" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
+        <v>535</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="K22" s="9">
+        <v>56016</v>
+      </c>
+      <c r="L22" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>536</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="J23" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="K23" s="9">
+        <v>45222</v>
+      </c>
+      <c r="L23" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>537</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="J24" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="K24" s="9">
+        <v>10597</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
+        <v>538</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="J25" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="K25" s="9">
+        <v>39581</v>
+      </c>
+      <c r="L25" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="J26" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="K26" s="9">
+        <v>5069</v>
+      </c>
+      <c r="L26" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>540</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="J27" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="K27" s="9">
+        <v>28723</v>
+      </c>
+      <c r="L27" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
+        <v>541</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="J28" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="K28" s="9">
+        <v>38478</v>
+      </c>
+      <c r="L28" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>542</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="J29" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="K29" s="9">
+        <v>28144</v>
+      </c>
+      <c r="L29" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>543</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="J30" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="K30" s="9">
+        <v>40062</v>
+      </c>
+      <c r="L30" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="7" t="s">
+        <v>544</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="J31" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K31" s="9">
+        <v>35073</v>
+      </c>
+      <c r="L31" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="J32" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="K32" s="9">
+        <v>24464</v>
+      </c>
+      <c r="L32" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>546</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="J33" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="K33" s="9">
+        <v>19529</v>
+      </c>
+      <c r="L33" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="7" t="s">
+        <v>547</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="J34" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="K34" s="9">
+        <v>44645</v>
+      </c>
+      <c r="L34" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>548</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="J35" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="K35" s="9">
+        <v>95120</v>
+      </c>
+      <c r="L35" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
+        <v>549</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="H36" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="J36" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="K36" s="9">
+        <v>43548</v>
+      </c>
+      <c r="L36" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="7" t="s">
+        <v>550</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>325</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="J37" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="K37" s="9">
+        <v>31790</v>
+      </c>
+      <c r="L37" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
+        <v>551</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>329</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>333</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="J38" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="K38" s="9">
+        <v>11531</v>
+      </c>
+      <c r="L38" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
+        <v>552</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>341</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="J39" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="K39" s="9">
+        <v>61468</v>
+      </c>
+      <c r="L39" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="7" t="s">
+        <v>553</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="H40" s="6" t="s">
+        <v>350</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="J40" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="K40" s="9">
+        <v>20223</v>
+      </c>
+      <c r="L40" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
+        <v>554</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>353</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>358</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="J41" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="K41" s="9">
+        <v>48636</v>
+      </c>
+      <c r="L41" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>555</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>361</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>362</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>364</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="H42" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>367</v>
+      </c>
+      <c r="J42" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="K42" s="9">
+        <v>30140</v>
+      </c>
+      <c r="L42" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="7" t="s">
+        <v>556</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>369</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>371</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>372</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="H43" s="6" t="s">
+        <v>374</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="J43" s="8" t="s">
+        <v>376</v>
+      </c>
+      <c r="K43" s="9">
+        <v>85381</v>
+      </c>
+      <c r="L43" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
+        <v>557</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>378</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>380</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>381</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>382</v>
+      </c>
+      <c r="H44" s="6" t="s">
+        <v>383</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="J44" s="8" t="s">
+        <v>385</v>
+      </c>
+      <c r="K44" s="9">
+        <v>57073</v>
+      </c>
+      <c r="L44" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
+        <v>558</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>387</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>388</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="G45" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="H45" s="6" t="s">
+        <v>392</v>
+      </c>
+      <c r="I45" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J45" s="8" t="s">
+        <v>393</v>
+      </c>
+      <c r="K45" s="9">
+        <v>65612</v>
+      </c>
+      <c r="L45" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="7" t="s">
+        <v>559</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>394</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>396</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>398</v>
+      </c>
+      <c r="G46" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="H46" s="6" t="s">
+        <v>400</v>
+      </c>
+      <c r="I46" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="J46" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="K46" s="9">
+        <v>67448</v>
+      </c>
+      <c r="L46" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="s">
+        <v>560</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>403</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>404</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>406</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="H47" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="I47" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="J47" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="K47" s="9">
+        <v>59405</v>
+      </c>
+      <c r="L47" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
+        <v>561</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>410</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>411</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>412</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>413</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>414</v>
+      </c>
+      <c r="G48" s="6" t="s">
+        <v>415</v>
+      </c>
+      <c r="H48" s="6" t="s">
+        <v>416</v>
+      </c>
+      <c r="I48" s="5" t="s">
+        <v>417</v>
+      </c>
+      <c r="J48" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="K48" s="9">
+        <v>92563</v>
+      </c>
+      <c r="L48" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="7" t="s">
+        <v>562</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>419</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>420</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>421</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>422</v>
+      </c>
+      <c r="G49" s="6" t="s">
+        <v>423</v>
+      </c>
+      <c r="H49" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="I49" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="J49" s="8" t="s">
+        <v>426</v>
+      </c>
+      <c r="K49" s="9">
+        <v>94271</v>
+      </c>
+      <c r="L49" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
+        <v>563</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>428</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>429</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>430</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>431</v>
+      </c>
+      <c r="G50" s="6" t="s">
+        <v>432</v>
+      </c>
+      <c r="H50" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="J50" s="8" t="s">
+        <v>435</v>
+      </c>
+      <c r="K50" s="9">
+        <v>77230</v>
+      </c>
+      <c r="L50" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="4" t="s">
+        <v>564</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>439</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>440</v>
+      </c>
+      <c r="G51" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="H51" s="6" t="s">
+        <v>442</v>
+      </c>
+      <c r="I51" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="J51" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="K51" s="9">
+        <v>34712</v>
+      </c>
+      <c r="L51" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L51"/>
+  <sheetViews>
+    <sheetView topLeftCell="A43" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="17.28515625" style="3" collapsed="1"/>
+    <col min="5" max="5" width="25.85546875" style="3" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.28515625" style="3" collapsed="1"/>
+    <col min="7" max="7" width="27.42578125" style="3" customWidth="1" collapsed="1"/>
+    <col min="8" max="16384" width="17.28515625" style="3" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>465</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -2246,9 +4358,7 @@
       <c r="A3" s="4" t="s">
         <v>466</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="B3" s="5"/>
       <c r="C3" s="6" t="s">
         <v>25</v>
       </c>
@@ -2436,9 +4546,7 @@
       <c r="A8" s="4" t="s">
         <v>471</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>69</v>
-      </c>
+      <c r="B8" s="5"/>
       <c r="C8" s="6" t="s">
         <v>70</v>
       </c>
@@ -2512,9 +4620,7 @@
       <c r="A10" s="7" t="s">
         <v>473</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>87</v>
-      </c>
+      <c r="B10" s="5"/>
       <c r="C10" s="6" t="s">
         <v>88</v>
       </c>
@@ -2622,7 +4728,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>476</v>
       </c>
@@ -2698,7 +4804,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>478</v>
       </c>
@@ -2774,7 +4880,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>480</v>
       </c>
@@ -3044,9 +5150,7 @@
       <c r="A24" s="4" t="s">
         <v>487</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>207</v>
-      </c>
+      <c r="B24" s="5"/>
       <c r="C24" s="6" t="s">
         <v>208</v>
       </c>
@@ -3382,7 +5486,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>496</v>
       </c>
@@ -3496,7 +5600,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>499</v>
       </c>
@@ -3652,9 +5756,7 @@
       <c r="A40" s="7" t="s">
         <v>503</v>
       </c>
-      <c r="B40" s="5" t="s">
-        <v>344</v>
-      </c>
+      <c r="B40" s="5"/>
       <c r="C40" s="6" t="s">
         <v>345</v>
       </c>
@@ -3766,9 +5868,7 @@
       <c r="A43" s="7" t="s">
         <v>506</v>
       </c>
-      <c r="B43" s="5" t="s">
-        <v>368</v>
-      </c>
+      <c r="B43" s="5"/>
       <c r="C43" s="6" t="s">
         <v>369</v>
       </c>
@@ -3880,9 +5980,7 @@
       <c r="A46" s="7" t="s">
         <v>509</v>
       </c>
-      <c r="B46" s="5" t="s">
-        <v>394</v>
-      </c>
+      <c r="B46" s="5"/>
       <c r="C46" s="6" t="s">
         <v>395</v>
       </c>
@@ -3952,13 +6050,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>511</v>
       </c>
-      <c r="B48" s="5" t="s">
-        <v>410</v>
-      </c>
+      <c r="B48" s="5"/>
       <c r="C48" s="6" t="s">
         <v>411</v>
       </c>
@@ -4032,9 +6128,7 @@
       <c r="A50" s="4" t="s">
         <v>513</v>
       </c>
-      <c r="B50" s="5" t="s">
-        <v>427</v>
-      </c>
+      <c r="B50" s="5"/>
       <c r="C50" s="6" t="s">
         <v>428</v>
       </c>

</xml_diff>

<commit_message>
TestNG.xml and SiginInTest commit
</commit_message>
<xml_diff>
--- a/FinalProject/data/pet-store-data.xlsx
+++ b/FinalProject/data/pet-store-data.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowHeight="6720" windowWidth="21225" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21225" windowHeight="6720" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="cart_items" r:id="rId1" sheetId="1"/>
-    <sheet name="users" r:id="rId2" sheetId="2"/>
-    <sheet name="users_without_password" r:id="rId3" sheetId="3"/>
+    <sheet name="cart_items" sheetId="1" r:id="rId1"/>
+    <sheet name="users" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:H20"/>
+  <oleSize ref="A1:J12"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1237" uniqueCount="665">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="465">
   <si>
     <t>ITEM_ID</t>
   </si>
@@ -1412,613 +1411,12 @@
   </si>
   <si>
     <t>https://petstore.octoperf.com/actions/Catalog.action?viewItem=&amp;itemId=EST-13</t>
-  </si>
-  <si>
-    <t>ABbpPrZJgWLHecLjJl5dy</t>
-  </si>
-  <si>
-    <t>mnrR8JB_klTm8DZM5eTls</t>
-  </si>
-  <si>
-    <t>VxFjJMN-eI9Byvu3nZYZW</t>
-  </si>
-  <si>
-    <t>s32MkZ7vTlqeUz4URVHQE</t>
-  </si>
-  <si>
-    <t>rlZJ0S6ymM9wC66CbuoAh</t>
-  </si>
-  <si>
-    <t>YjbJFYZzc_dd1cobMiWu_</t>
-  </si>
-  <si>
-    <t>GvLSJj_WuROsX8Tnv0rEA</t>
-  </si>
-  <si>
-    <t>XftNPrpXSW0Qc_Mc1fmfe</t>
-  </si>
-  <si>
-    <t>VFNdKXfoa3P9XsGwpaXGP</t>
-  </si>
-  <si>
-    <t>ggJt4SlVDK-TUsTMjyb5K</t>
-  </si>
-  <si>
-    <t>ogiX32BJopnUFW4iw3j57</t>
-  </si>
-  <si>
-    <t>v4s6alZ_tMh4fq7MPufCV</t>
-  </si>
-  <si>
-    <t>5a4cbTAu30-C0QQtioxTV</t>
-  </si>
-  <si>
-    <t>-mia5tcLoEhe8JVCmrJiV</t>
-  </si>
-  <si>
-    <t>HFRnFi145Ak9D0Ue5XrbH</t>
-  </si>
-  <si>
-    <t>vs1-HYNusjhj62iRLjOQw</t>
-  </si>
-  <si>
-    <t>WraAVP6-O-w801i6c2HO1</t>
-  </si>
-  <si>
-    <t>XN7kiVCQWbKed76nBk7VH</t>
-  </si>
-  <si>
-    <t>EXI2L7zZbJr3ao57w7lQf</t>
-  </si>
-  <si>
-    <t>1bmisEZ0wifiGV2pNxexH</t>
-  </si>
-  <si>
-    <t>xZ0iVVcipbchwoqcA66WD</t>
-  </si>
-  <si>
-    <t>QuZdoi1k0Mi8xkFGHkun4</t>
-  </si>
-  <si>
-    <t>vLPfi5t4Y31o5NJP3YUzX</t>
-  </si>
-  <si>
-    <t>JlGhuUJlhNeWsNlQr5sX9</t>
-  </si>
-  <si>
-    <t>Vqe4D8gmvhPsFJ3q1ucFe</t>
-  </si>
-  <si>
-    <t>SkMzxT9_hxladNwW5s3cn</t>
-  </si>
-  <si>
-    <t>yXMM4LOU-UL4PUBQku5GY</t>
-  </si>
-  <si>
-    <t>zQ8KAFrq0cbSho2VXJVCp</t>
-  </si>
-  <si>
-    <t>EU3HT_I4rrgh_Yc5TjJyK</t>
-  </si>
-  <si>
-    <t>Br1AU8vbkd2ZVTK2LYHR_</t>
-  </si>
-  <si>
-    <t>1Ccle0PAD2qQM6hLmjQlD</t>
-  </si>
-  <si>
-    <t>RSSlXeY5cGICHkNEOa0gA</t>
-  </si>
-  <si>
-    <t>UfcHZqro2yPi72496hTaO</t>
-  </si>
-  <si>
-    <t>PPmAtOwjZRoFBNpGy-wuq</t>
-  </si>
-  <si>
-    <t>tOYiw-PvKQfE25nyIKJNP</t>
-  </si>
-  <si>
-    <t>TDTWVKfm--yRq65QVGvJ6</t>
-  </si>
-  <si>
-    <t>9EUJznKj-asTUtS_jDnMZ</t>
-  </si>
-  <si>
-    <t>5PRJfR8-nAPazZs9o8MaP</t>
-  </si>
-  <si>
-    <t>I8_0BD13TcOWAYk745JMs</t>
-  </si>
-  <si>
-    <t>ogOleczG-X4pt8NepM6AR</t>
-  </si>
-  <si>
-    <t>hLZhZdmR1ARqGXvkgFagg</t>
-  </si>
-  <si>
-    <t>jXbvII0IVe1WCHw5Hf-Wc</t>
-  </si>
-  <si>
-    <t>v9iuWQ3FaSgZ0XufCUGvC</t>
-  </si>
-  <si>
-    <t>ZYAY5CGix06gc6z6fT-wC</t>
-  </si>
-  <si>
-    <t>jwts_HfppIm4DJN-oWAeA</t>
-  </si>
-  <si>
-    <t>mF6pviiRrtkKF4e-wsqRh</t>
-  </si>
-  <si>
-    <t>TUd8fEwjuggbkYAj361xS</t>
-  </si>
-  <si>
-    <t>AnbaKNjMCCiNhivViWppO</t>
-  </si>
-  <si>
-    <t>vmpzk8TYITOSUzZj_xgyB</t>
-  </si>
-  <si>
-    <t>hrqn7qAinDQwBHuGQebAb</t>
-  </si>
-  <si>
-    <t>eH0IrLwD37oLQuIt9UZsH</t>
-  </si>
-  <si>
-    <t>eUmLcHrOxRF37jI1UAM1t</t>
-  </si>
-  <si>
-    <t>LotA1DbhYQSwvI1yqPU4L</t>
-  </si>
-  <si>
-    <t>B2KA_hiyIYAR9KzfhN0L4</t>
-  </si>
-  <si>
-    <t>ogmWyovezRITiXYwmFewx</t>
-  </si>
-  <si>
-    <t>5ZOWxhjG40iXsBHSlD65V</t>
-  </si>
-  <si>
-    <t>gJcu7zL1pxt8PYU2EU76M</t>
-  </si>
-  <si>
-    <t>lKUlBD72YkoBcIUv3VfRK</t>
-  </si>
-  <si>
-    <t>38RugvUNBydvTlmheTvT8</t>
-  </si>
-  <si>
-    <t>lI267LtIvkDsu3LtbVxU2</t>
-  </si>
-  <si>
-    <t>qd90bl1vNijZIzy-T6Tkk</t>
-  </si>
-  <si>
-    <t>fbplhm552lpsDoos-F81d</t>
-  </si>
-  <si>
-    <t>JCgt3RANHC_Ts3aTahySI</t>
-  </si>
-  <si>
-    <t>zWuiekBlFTATKJohoR_WD</t>
-  </si>
-  <si>
-    <t>9pLrqfmwvuCFSxgQ1R2L5</t>
-  </si>
-  <si>
-    <t>Pk3XcezcGRdtu7VIk0VUD</t>
-  </si>
-  <si>
-    <t>hsLToIR1JY-vxIrppZWKf</t>
-  </si>
-  <si>
-    <t>_nhcqYWbrEc6X3nbICmmA</t>
-  </si>
-  <si>
-    <t>doWtq9K9BSNlCBobFGLtH</t>
-  </si>
-  <si>
-    <t>fh92EbG9WN6F90eyRhHAw</t>
-  </si>
-  <si>
-    <t>tJ3lvCHnBNqPt3QSCqOuP</t>
-  </si>
-  <si>
-    <t>j4C2oI8ZF9BOTabkvmOiH</t>
-  </si>
-  <si>
-    <t>R9UfX3cffu82RwM-6o0Mh</t>
-  </si>
-  <si>
-    <t>Pg1YOFuFdr9neiafFVgmv</t>
-  </si>
-  <si>
-    <t>NYgxewKag8ZaeBljrD0Py</t>
-  </si>
-  <si>
-    <t>DdJpCwHRuNRQvduc2PG7v</t>
-  </si>
-  <si>
-    <t>v3to55rnqkCut6kD27sCK</t>
-  </si>
-  <si>
-    <t>5nbWXy-Rls4fC5-4vpC3u</t>
-  </si>
-  <si>
-    <t>lVXduHpSclHoEl81NzG1Y</t>
-  </si>
-  <si>
-    <t>l_N7U1Z3DJCQdPVdZ-2rK</t>
-  </si>
-  <si>
-    <t>HiB8pPMk0FV3OwSqgdw8r</t>
-  </si>
-  <si>
-    <t>RYY0WUjxcKs85ZRLR2xQk</t>
-  </si>
-  <si>
-    <t>gUommyV3l5qmLWgJFMj_t</t>
-  </si>
-  <si>
-    <t>GV8Uv9cK43JDpVApUT-Mt</t>
-  </si>
-  <si>
-    <t>-ONfkNqgUktCDACHGOOzB</t>
-  </si>
-  <si>
-    <t>9R9CR_Y2YhjwfYSwfifYp</t>
-  </si>
-  <si>
-    <t>bQphyd-yBvpxPx5shyAA_</t>
-  </si>
-  <si>
-    <t>5CL0vUAHd2ZkyM4bhfSLY</t>
-  </si>
-  <si>
-    <t>quYtV0J3lLarex2meO-Ic</t>
-  </si>
-  <si>
-    <t>2vybb9QpBjKwMFIU7myhq</t>
-  </si>
-  <si>
-    <t>tcfZV3CjHo-_mjbMBDslw</t>
-  </si>
-  <si>
-    <t>r6zIYSEhK2sUDS9tcMSec</t>
-  </si>
-  <si>
-    <t>MyJyK1MWSXVJZz6tgNLMf</t>
-  </si>
-  <si>
-    <t>HP-HVAXLT-7PJs5UIIUWc</t>
-  </si>
-  <si>
-    <t>SOp3CKHqNFm5HKlTJMPAO</t>
-  </si>
-  <si>
-    <t>EpVs80DYUki6wPoGk0kF4</t>
-  </si>
-  <si>
-    <t>pwyEbcbN6_gy11uhgz8uF</t>
-  </si>
-  <si>
-    <t>xa2ciMjPr7IkoC6lHxmoF</t>
-  </si>
-  <si>
-    <t>7IMjkSglqHmXrKHwRdu3O</t>
-  </si>
-  <si>
-    <t>ImWUAe6XeCtnEhCyNbfoF</t>
-  </si>
-  <si>
-    <t>KOr2g5a-kRZ0zCFb-jdc1</t>
-  </si>
-  <si>
-    <t>a-j7uxhDbrnsFm_O9Z4Q1</t>
-  </si>
-  <si>
-    <t>Eey4h2UJ6wwVzbVz-C_M-</t>
-  </si>
-  <si>
-    <t>5t9U044r6b_1yWEWlKush</t>
-  </si>
-  <si>
-    <t>vtjdT0AJlodnIMJfaCaQ4</t>
-  </si>
-  <si>
-    <t>Q4nKHAMIPzxyVFNIFehXp</t>
-  </si>
-  <si>
-    <t>CLmLNghFbuEvJQQiL3tYV</t>
-  </si>
-  <si>
-    <t>rt0JxUq7Qlf4XYOC3-A6t</t>
-  </si>
-  <si>
-    <t>JKyawi3YdfHxZ3XCSz7QD</t>
-  </si>
-  <si>
-    <t>sVBF9jt56CAXPc-2CUTRO</t>
-  </si>
-  <si>
-    <t>xJ3Hnj4sBXDVNLYyEv7Cb</t>
-  </si>
-  <si>
-    <t>tJ2bYSYXWvOdnsK6QtMI0</t>
-  </si>
-  <si>
-    <t>y-glnc00ZYe4Y-j92Z_Dh</t>
-  </si>
-  <si>
-    <t>j1S2JAdZ1azcL8tboc7sG</t>
-  </si>
-  <si>
-    <t>CVFcu1nn_i9muvqthxWO5</t>
-  </si>
-  <si>
-    <t>YGI-0Z1_57jKYVKiRjaB-</t>
-  </si>
-  <si>
-    <t>auM6xEdZBVJnBA7_VgvaV</t>
-  </si>
-  <si>
-    <t>aycv0JaLNuhpSiNN60VZ1</t>
-  </si>
-  <si>
-    <t>lcuoU02W_74C8AtJ8bUgp</t>
-  </si>
-  <si>
-    <t>W-aRsbsJFfqXBThGVnusb</t>
-  </si>
-  <si>
-    <t>BZB4VaCAIwX6kdBD0AUq5</t>
-  </si>
-  <si>
-    <t>ypInKFjyJJYk1vlUTCFvm</t>
-  </si>
-  <si>
-    <t>VkLErW1q7eKdpPgdEZF18</t>
-  </si>
-  <si>
-    <t>PqTw1znzF9Q76Nfxv94-U</t>
-  </si>
-  <si>
-    <t>i_elVyPFVSihs9EPmbxqt</t>
-  </si>
-  <si>
-    <t>GyuLAJPveI16bxvRznG7R</t>
-  </si>
-  <si>
-    <t>3i13nF_mcNkk25EacbGC5</t>
-  </si>
-  <si>
-    <t>w6wpIvboptwCAE2JQO2pD</t>
-  </si>
-  <si>
-    <t>fx5LD9PfLbuuo6EngMxCD</t>
-  </si>
-  <si>
-    <t>7KZ61CocLhEXn0IcCZPuL</t>
-  </si>
-  <si>
-    <t>UEUfOucgHrpt_OPB_pOhC</t>
-  </si>
-  <si>
-    <t>D_GvWb9a519a0wtFaHF4x</t>
-  </si>
-  <si>
-    <t>Fq391eEmUSM3byfelaOe_</t>
-  </si>
-  <si>
-    <t>WIHKslV5mFxIiPculdEIJ</t>
-  </si>
-  <si>
-    <t>l2TtKKzzvZxptkHcC3XUw</t>
-  </si>
-  <si>
-    <t>9uET5TRcb5sLjR41VfqCq</t>
-  </si>
-  <si>
-    <t>stz6-aEaD7hJtSrDTy5Zc</t>
-  </si>
-  <si>
-    <t>-ApLhlHbpU1WonpbP_4D6</t>
-  </si>
-  <si>
-    <t>9ShLZ4EQk93Yzksa6LBbC</t>
-  </si>
-  <si>
-    <t>xjdRfsh_UJEudPpgxiqBa</t>
-  </si>
-  <si>
-    <t>oUxs_aStgrVvH6EDkVubt</t>
-  </si>
-  <si>
-    <t>EWyyX34AkZsQCoMJnKJ6n</t>
-  </si>
-  <si>
-    <t>kNn4gKnrlc0-rc3163Fxx</t>
-  </si>
-  <si>
-    <t>LTwDdypKKrOMhf0PU6Zfy</t>
-  </si>
-  <si>
-    <t>2Bm0NyU7llsq9mJAiCjBS</t>
-  </si>
-  <si>
-    <t>21X06qKXyIne8b9-hWW4l</t>
-  </si>
-  <si>
-    <t>tQKjpBHlmQCGJ_1Npz4f2</t>
-  </si>
-  <si>
-    <t>uWCRG8A5cfuzGfs6exD-u</t>
-  </si>
-  <si>
-    <t>EJOVkOfVfhC2PSNU87i6L</t>
-  </si>
-  <si>
-    <t>aDdftgGaFzuUylG_xZMYU</t>
-  </si>
-  <si>
-    <t>foC-Hw8NPr1C2eR6reIGf</t>
-  </si>
-  <si>
-    <t>wx4hW5eEbb2NMzN-xIlKC</t>
-  </si>
-  <si>
-    <t>IYuFI1wQzZc7vf5SQ94CE</t>
-  </si>
-  <si>
-    <t>y_lSNCasm-_djbXGeB3HR</t>
-  </si>
-  <si>
-    <t>mISvDHVoHi4s_HHHGTDPG</t>
-  </si>
-  <si>
-    <t>CcDwjjXMFsEwdgWRsZHrm</t>
-  </si>
-  <si>
-    <t>aKs4iVAgP_mEGFduybANU</t>
-  </si>
-  <si>
-    <t>Uokkm_Qhrjj3m4Ra0pAcg</t>
-  </si>
-  <si>
-    <t>AtZsmIu7sj65UzQsBhB49</t>
-  </si>
-  <si>
-    <t>3tHxwGsYK15IIjvZ7K1_o</t>
-  </si>
-  <si>
-    <t>diLBul_6dgORxSyh6Mcan</t>
-  </si>
-  <si>
-    <t>ZmfzweNHYk4K8lm0y89H5</t>
-  </si>
-  <si>
-    <t>30D7ndoXF6lwJjrBAjLoJ</t>
-  </si>
-  <si>
-    <t>x8gFS-8ALaJLMqcentDiu</t>
-  </si>
-  <si>
-    <t>XcgYjF_lfFSvTcECAFCNy</t>
-  </si>
-  <si>
-    <t>XUpQ4Z97DdBTvmxn3W_NK</t>
-  </si>
-  <si>
-    <t>BgPyf20uxt_NDA89WxMgq</t>
-  </si>
-  <si>
-    <t>ZmGse9GDIQ5yE-o542Kab</t>
-  </si>
-  <si>
-    <t>R8JBZrA1aJJiWXV8DWXD1</t>
-  </si>
-  <si>
-    <t>49ep6iH6_IEIxM5NUpOSz</t>
-  </si>
-  <si>
-    <t>jtcANAsfdR30irzL6oWVv</t>
-  </si>
-  <si>
-    <t>IrClY-OANceqURYkIoDa8</t>
-  </si>
-  <si>
-    <t>9oSPEYr8UzYVQ57fj0P_x</t>
-  </si>
-  <si>
-    <t>LIcjbTwnXYDDfegPngsYQ</t>
-  </si>
-  <si>
-    <t>SYnm38DKb-gY4CV4gRLlj</t>
-  </si>
-  <si>
-    <t>SqfIzkqVecdsfWTWD64BI</t>
-  </si>
-  <si>
-    <t>bU2XlbQi1JqNVRVCmx5lR</t>
-  </si>
-  <si>
-    <t>4Lu9xkmhc5QkeEDXIeayK</t>
-  </si>
-  <si>
-    <t>YNZMf4Bp6433ioAFh2v8c</t>
-  </si>
-  <si>
-    <t>V8NuPIF66noNHDbLAu9Cv</t>
-  </si>
-  <si>
-    <t>BQIuo8Gs5a20KkFFM4-r0</t>
-  </si>
-  <si>
-    <t>owOuO-wTR8j4SeQ2tz8e4</t>
-  </si>
-  <si>
-    <t>1r6CJ2nZlr-Yj9sL7fq6L</t>
-  </si>
-  <si>
-    <t>uL7XmyoALrQriwjeZDmRu</t>
-  </si>
-  <si>
-    <t>wPr3kCdL_nKC0MsJDUSWD</t>
-  </si>
-  <si>
-    <t>xri5gsWBS-y4xrPD5hXKJ</t>
-  </si>
-  <si>
-    <t>J0rCIquPhPDDLadLR1bBU</t>
-  </si>
-  <si>
-    <t>2vVakBdRLU4WEi8APnUA0</t>
-  </si>
-  <si>
-    <t>P92gL6dG3IgPqtiAxYgT1</t>
-  </si>
-  <si>
-    <t>2jSZZiGUb3gua1-xaf82H</t>
-  </si>
-  <si>
-    <t>Z6ep-STSsnjuvhaCRDII3</t>
-  </si>
-  <si>
-    <t>ppWUY04qYArYI28b3RPtl</t>
-  </si>
-  <si>
-    <t>PkQ7FE7s-tqPyHIU3HCFH</t>
-  </si>
-  <si>
-    <t>ZME_pnMUHvRWySq5L0rZA</t>
-  </si>
-  <si>
-    <t>xzFH495aZeTWIMCdRx8Wj</t>
-  </si>
-  <si>
-    <t>QRP6VVOzhjArvADtdQtu0</t>
-  </si>
-  <si>
-    <t>UGEic9ik4ChVAdpkOxaHr</t>
-  </si>
-  <si>
-    <t>ScTzlca0u38x47W_nEFPp</t>
-  </si>
-  <si>
-    <t>H2N10_i_g5_cRMLR9b9sz</t>
-  </si>
-  <si>
-    <t>OqLKydfct2Ju_XJ9j1zF4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2140,52 +1538,52 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="14">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="5" fontId="5" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="6" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyProtection="1" borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2202,10 +1600,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -2240,7 +1638,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2275,7 +1673,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2363,7 +1761,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -2372,13 +1770,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -2388,7 +1786,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -2397,7 +1795,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -2406,7 +1804,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -2416,12 +1814,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -2452,7 +1850,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -2471,7 +1869,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -2483,17 +1881,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="28.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="108.0" collapsed="true"/>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
+    <col min="2" max="2" width="108" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -2586,39 +1984,39 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2"/>
-    <hyperlink r:id="rId2" ref="B3"/>
-    <hyperlink r:id="rId3" ref="B4"/>
-    <hyperlink r:id="rId4" ref="B5"/>
-    <hyperlink r:id="rId5" ref="B6"/>
-    <hyperlink r:id="rId6" ref="B7"/>
-    <hyperlink r:id="rId7" ref="B8"/>
-    <hyperlink r:id="rId8" ref="B9"/>
-    <hyperlink r:id="rId9" ref="B10"/>
-    <hyperlink r:id="rId10" ref="B11"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="B7" r:id="rId6"/>
+    <hyperlink ref="B8" r:id="rId7"/>
+    <hyperlink ref="B9" r:id="rId8"/>
+    <hyperlink ref="B10" r:id="rId9"/>
+    <hyperlink ref="B11" r:id="rId10"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScaleNormal="85">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" style="3" width="17.28515625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="3" width="25.85546875" collapsed="true"/>
-    <col min="6" max="6" style="3" width="17.28515625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="3" width="27.42578125" collapsed="true"/>
-    <col min="8" max="16384" style="3" width="17.28515625" collapsed="true"/>
+    <col min="1" max="4" width="17.28515625" style="3"/>
+    <col min="5" max="5" width="25.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" style="3"/>
+    <col min="7" max="7" width="27.42578125" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="17.28515625" style="3"/>
   </cols>
   <sheetData>
-    <row ht="15.75" r="1" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2656,9 +2054,9 @@
         <v>13</v>
       </c>
     </row>
-    <row ht="29.25" r="2" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>615</v>
+    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
+        <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>14</v>
@@ -2694,9 +2092,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="30" r="3" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>616</v>
+    <row r="3" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>24</v>
@@ -2732,9 +2130,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="30" r="4" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>617</v>
+    <row r="4" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>33</v>
@@ -2770,9 +2168,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="30" r="5" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>618</v>
+    <row r="5" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>42</v>
@@ -2808,9 +2206,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="29.25" r="6" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>619</v>
+    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>51</v>
@@ -2846,9 +2244,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="30" r="7" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
-        <v>620</v>
+    <row r="7" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7">
+        <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>60</v>
@@ -2884,9 +2282,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="29.25" r="8" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>621</v>
+    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
+        <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>69</v>
@@ -2922,9 +2320,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="30" r="9" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>622</v>
+    <row r="9" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
+        <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>78</v>
@@ -2960,9 +2358,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="30" r="10" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
-        <v>623</v>
+    <row r="10" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
+        <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>87</v>
@@ -2998,9 +2396,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="30" r="11" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>624</v>
+    <row r="11" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
+        <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>96</v>
@@ -3036,9 +2434,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="30" r="12" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>625</v>
+    <row r="12" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
+        <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>105</v>
@@ -3074,9 +2472,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="30" r="13" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
-        <v>626</v>
+    <row r="13" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
+        <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>114</v>
@@ -3112,9 +2510,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="29.25" r="14" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>627</v>
+    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
+        <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>123</v>
@@ -3150,9 +2548,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="30" r="15" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
-        <v>628</v>
+    <row r="15" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4">
+        <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>131</v>
@@ -3188,9 +2586,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="30" r="16" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
-        <v>629</v>
+    <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="7">
+        <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>139</v>
@@ -3226,9 +2624,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="30" r="17" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
-        <v>630</v>
+    <row r="17" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4">
+        <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>148</v>
@@ -3264,9 +2662,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="29.25" r="18" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
-        <v>631</v>
+    <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="4">
+        <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>156</v>
@@ -3302,9 +2700,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="30" r="19" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
-        <v>632</v>
+    <row r="19" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="7">
+        <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>165</v>
@@ -3340,9 +2738,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="29.25" r="20" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
-        <v>633</v>
+    <row r="20" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="4">
+        <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>173</v>
@@ -3378,9 +2776,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="29.25" r="21" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
-        <v>634</v>
+    <row r="21" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
+        <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>181</v>
@@ -3416,9 +2814,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="30" r="22" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
-        <v>635</v>
+    <row r="22" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="7">
+        <v>21</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>190</v>
@@ -3454,9 +2852,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="30" r="23" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
-        <v>636</v>
+    <row r="23" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="4">
+        <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>199</v>
@@ -3492,9 +2890,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="29.25" r="24" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
-        <v>637</v>
+    <row r="24" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="4">
+        <v>23</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>207</v>
@@ -3530,9 +2928,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="30" r="25" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
-        <v>638</v>
+    <row r="25" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="7">
+        <v>24</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>216</v>
@@ -3568,9 +2966,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="29.25" r="26" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
-        <v>639</v>
+    <row r="26" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="4">
+        <v>25</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>225</v>
@@ -3606,9 +3004,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="30" r="27" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
-        <v>640</v>
+    <row r="27" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="4">
+        <v>26</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>234</v>
@@ -3644,9 +3042,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="30" r="28" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="7" t="s">
-        <v>641</v>
+    <row r="28" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="7">
+        <v>27</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>243</v>
@@ -3682,9 +3080,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="30" r="29" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
-        <v>642</v>
+    <row r="29" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="4">
+        <v>28</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>251</v>
@@ -3720,9 +3118,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="30" r="30" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
-        <v>643</v>
+    <row r="30" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="4">
+        <v>29</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>259</v>
@@ -3758,9 +3156,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="30" r="31" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="7" t="s">
-        <v>644</v>
+    <row r="31" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="7">
+        <v>30</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>268</v>
@@ -3796,9 +3194,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="29.25" r="32" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
-        <v>645</v>
+    <row r="32" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="4">
+        <v>31</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>276</v>
@@ -3834,9 +3232,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="30" r="33" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="s">
-        <v>646</v>
+    <row r="33" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="4">
+        <v>32</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>284</v>
@@ -3872,9 +3270,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="30" r="34" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="7" t="s">
-        <v>647</v>
+    <row r="34" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="7">
+        <v>33</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>292</v>
@@ -3910,9 +3308,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="30" r="35" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="4" t="s">
-        <v>648</v>
+    <row r="35" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="4">
+        <v>34</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>301</v>
@@ -3948,9 +3346,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="43.5" r="36" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="4" t="s">
-        <v>649</v>
+    <row r="36" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="4">
+        <v>35</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>310</v>
@@ -3986,9 +3384,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="30" r="37" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="7" t="s">
-        <v>650</v>
+    <row r="37" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="7">
+        <v>36</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>319</v>
@@ -4024,9 +3422,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="43.5" r="38" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="4" t="s">
-        <v>651</v>
+    <row r="38" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="4">
+        <v>37</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>327</v>
@@ -4062,9 +3460,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="30" r="39" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="4" t="s">
-        <v>652</v>
+    <row r="39" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="4">
+        <v>38</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>336</v>
@@ -4100,9 +3498,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="30" r="40" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="7" t="s">
-        <v>653</v>
+    <row r="40" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="7">
+        <v>39</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>344</v>
@@ -4138,9 +3536,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="30" r="41" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="4" t="s">
-        <v>654</v>
+    <row r="41" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="4">
+        <v>40</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>352</v>
@@ -4176,9 +3574,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="30" r="42" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="4" t="s">
-        <v>655</v>
+    <row r="42" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="4">
+        <v>41</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>360</v>
@@ -4214,9 +3612,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="30" r="43" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="7" t="s">
-        <v>656</v>
+    <row r="43" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="7">
+        <v>42</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>368</v>
@@ -4252,9 +3650,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="30" r="44" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="4" t="s">
-        <v>657</v>
+    <row r="44" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="4">
+        <v>43</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>377</v>
@@ -4290,9 +3688,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="30" r="45" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="4" t="s">
-        <v>658</v>
+    <row r="45" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="4">
+        <v>44</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>386</v>
@@ -4328,9 +3726,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="30" r="46" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="7" t="s">
-        <v>659</v>
+    <row r="46" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="7">
+        <v>45</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>394</v>
@@ -4366,9 +3764,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="30" r="47" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="4" t="s">
-        <v>660</v>
+    <row r="47" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="4">
+        <v>46</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>402</v>
@@ -4404,9 +3802,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="29.25" r="48" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="4" t="s">
-        <v>661</v>
+    <row r="48" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="4">
+        <v>47</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>410</v>
@@ -4442,9 +3840,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="30" r="49" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="7" t="s">
-        <v>662</v>
+    <row r="49" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="7">
+        <v>48</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>418</v>
@@ -4480,9 +3878,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="30" r="50" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="4" t="s">
-        <v>663</v>
+    <row r="50" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="4">
+        <v>49</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>427</v>
@@ -4518,9 +3916,9 @@
         <v>23</v>
       </c>
     </row>
-    <row ht="30" r="51" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="4" t="s">
-        <v>664</v>
+    <row r="51" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="4">
+        <v>50</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>436</v>
@@ -4557,1950 +3955,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M51"/>
-  <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0" zoomScaleNormal="85">
-      <selection activeCell="E52" sqref="E52"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="4" style="3" width="17.28515625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="3" width="25.85546875" collapsed="true"/>
-    <col min="6" max="6" style="3" width="17.28515625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="3" width="27.42578125" collapsed="true"/>
-    <col min="8" max="16384" style="3" width="17.28515625" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row ht="15.75" r="1" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row ht="29.25" r="2" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>465</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" s="9">
-        <v>33101</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="30" r="3" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>466</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="K3" s="9">
-        <v>23308</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="30" r="4" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>467</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="K4" s="9">
-        <v>26739</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="30" r="5" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>468</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="K5" s="9">
-        <v>74468</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="29.25" r="6" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>469</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="K6" s="9">
-        <v>28160</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="30" r="7" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
-        <v>470</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="K7" s="9">
-        <v>15545</v>
-      </c>
-      <c r="L7" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="29.25" r="8" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>471</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="K8" s="9">
-        <v>65080</v>
-      </c>
-      <c r="L8" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="30" r="9" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>472</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="K9" s="9">
-        <v>82718</v>
-      </c>
-      <c r="L9" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="30" r="10" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
-        <v>473</v>
-      </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="K10" s="9">
-        <v>10273</v>
-      </c>
-      <c r="L10" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="30" r="11" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>474</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="K11" s="9">
-        <v>58651</v>
-      </c>
-      <c r="L11" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="30" r="12" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>475</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="K12" s="9">
-        <v>46851</v>
-      </c>
-      <c r="L12" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="30" r="13" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
-        <v>476</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="K13" s="9">
-        <v>15601</v>
-      </c>
-      <c r="L13" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="29.25" r="14" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>477</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="J14" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="K14" s="9">
-        <v>47992</v>
-      </c>
-      <c r="L14" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="43.5" r="15" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
-        <v>478</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="J15" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="K15" s="9">
-        <v>78338</v>
-      </c>
-      <c r="L15" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="30" r="16" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
-        <v>479</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="K16" s="9">
-        <v>76465</v>
-      </c>
-      <c r="L16" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="43.5" r="17" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
-        <v>480</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="J17" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="K17" s="9">
-        <v>38369</v>
-      </c>
-      <c r="L17" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="29.25" r="18" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
-        <v>481</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="J18" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="K18" s="9">
-        <v>18449</v>
-      </c>
-      <c r="L18" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="30" r="19" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
-        <v>482</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="J19" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="K19" s="9">
-        <v>52640</v>
-      </c>
-      <c r="L19" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="29.25" r="20" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
-        <v>483</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="J20" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="K20" s="9">
-        <v>15250</v>
-      </c>
-      <c r="L20" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="29.25" r="21" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
-        <v>484</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="H21" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="J21" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="K21" s="9">
-        <v>93718</v>
-      </c>
-      <c r="L21" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="30" r="22" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
-        <v>485</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="H22" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="J22" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="K22" s="9">
-        <v>56016</v>
-      </c>
-      <c r="L22" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="30" r="23" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
-        <v>486</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="H23" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="I23" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="J23" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="K23" s="9">
-        <v>45222</v>
-      </c>
-      <c r="L23" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="29.25" r="24" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
-        <v>487</v>
-      </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="H24" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="I24" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="J24" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="K24" s="9">
-        <v>10597</v>
-      </c>
-      <c r="L24" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="30" r="25" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
-        <v>488</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="H25" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="J25" s="8" t="s">
-        <v>224</v>
-      </c>
-      <c r="K25" s="9">
-        <v>39581</v>
-      </c>
-      <c r="L25" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="29.25" r="26" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
-        <v>489</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>227</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="H26" s="6" t="s">
-        <v>231</v>
-      </c>
-      <c r="I26" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="J26" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="K26" s="9">
-        <v>5069</v>
-      </c>
-      <c r="L26" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="30" r="27" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
-        <v>490</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>239</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="J27" s="8" t="s">
-        <v>242</v>
-      </c>
-      <c r="K27" s="9">
-        <v>28723</v>
-      </c>
-      <c r="L27" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="30" r="28" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="7" t="s">
-        <v>491</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>244</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>246</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="G28" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="H28" s="6" t="s">
-        <v>249</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="J28" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="K28" s="9">
-        <v>38478</v>
-      </c>
-      <c r="L28" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="30" r="29" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
-        <v>492</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>253</v>
-      </c>
-      <c r="E29" s="10" t="s">
-        <v>254</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>256</v>
-      </c>
-      <c r="H29" s="6" t="s">
-        <v>257</v>
-      </c>
-      <c r="I29" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="J29" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="K29" s="9">
-        <v>28144</v>
-      </c>
-      <c r="L29" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="30" r="30" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
-        <v>493</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>260</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>262</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="G30" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="H30" s="6" t="s">
-        <v>265</v>
-      </c>
-      <c r="I30" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="J30" s="8" t="s">
-        <v>267</v>
-      </c>
-      <c r="K30" s="9">
-        <v>40062</v>
-      </c>
-      <c r="L30" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="30" r="31" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="7" t="s">
-        <v>494</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>269</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>272</v>
-      </c>
-      <c r="G31" s="6" t="s">
-        <v>273</v>
-      </c>
-      <c r="H31" s="6" t="s">
-        <v>274</v>
-      </c>
-      <c r="I31" s="5" t="s">
-        <v>275</v>
-      </c>
-      <c r="J31" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="K31" s="9">
-        <v>35073</v>
-      </c>
-      <c r="L31" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="29.25" r="32" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
-        <v>495</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>277</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>278</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>279</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G32" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="H32" s="6" t="s">
-        <v>282</v>
-      </c>
-      <c r="I32" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="J32" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="K32" s="9">
-        <v>24464</v>
-      </c>
-      <c r="L32" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="30" r="33" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="s">
-        <v>496</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>285</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>286</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>287</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>288</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>289</v>
-      </c>
-      <c r="H33" s="6" t="s">
-        <v>290</v>
-      </c>
-      <c r="I33" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="J33" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="K33" s="9">
-        <v>19529</v>
-      </c>
-      <c r="L33" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="30" r="34" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="7" t="s">
-        <v>497</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>292</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>293</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>294</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>295</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>296</v>
-      </c>
-      <c r="G34" s="6" t="s">
-        <v>297</v>
-      </c>
-      <c r="H34" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="I34" s="5" t="s">
-        <v>299</v>
-      </c>
-      <c r="J34" s="8" t="s">
-        <v>300</v>
-      </c>
-      <c r="K34" s="9">
-        <v>44645</v>
-      </c>
-      <c r="L34" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="30" r="35" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="4" t="s">
-        <v>498</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>301</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>302</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>303</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>305</v>
-      </c>
-      <c r="G35" s="6" t="s">
-        <v>306</v>
-      </c>
-      <c r="H35" s="6" t="s">
-        <v>307</v>
-      </c>
-      <c r="I35" s="5" t="s">
-        <v>308</v>
-      </c>
-      <c r="J35" s="8" t="s">
-        <v>309</v>
-      </c>
-      <c r="K35" s="9">
-        <v>95120</v>
-      </c>
-      <c r="L35" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="43.5" r="36" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="4" t="s">
-        <v>499</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>310</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>311</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>312</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>313</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>314</v>
-      </c>
-      <c r="G36" s="6" t="s">
-        <v>315</v>
-      </c>
-      <c r="H36" s="6" t="s">
-        <v>316</v>
-      </c>
-      <c r="I36" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="J36" s="8" t="s">
-        <v>318</v>
-      </c>
-      <c r="K36" s="9">
-        <v>43548</v>
-      </c>
-      <c r="L36" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="30" r="37" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="7" t="s">
-        <v>500</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>320</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>321</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>322</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>323</v>
-      </c>
-      <c r="G37" s="6" t="s">
-        <v>324</v>
-      </c>
-      <c r="H37" s="6" t="s">
-        <v>325</v>
-      </c>
-      <c r="I37" s="5" t="s">
-        <v>326</v>
-      </c>
-      <c r="J37" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="K37" s="9">
-        <v>31790</v>
-      </c>
-      <c r="L37" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="30" r="38" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="4" t="s">
-        <v>501</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>327</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>328</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>329</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>330</v>
-      </c>
-      <c r="F38" s="6" t="s">
-        <v>331</v>
-      </c>
-      <c r="G38" s="6" t="s">
-        <v>332</v>
-      </c>
-      <c r="H38" s="6" t="s">
-        <v>333</v>
-      </c>
-      <c r="I38" s="5" t="s">
-        <v>334</v>
-      </c>
-      <c r="J38" s="8" t="s">
-        <v>335</v>
-      </c>
-      <c r="K38" s="9">
-        <v>11531</v>
-      </c>
-      <c r="L38" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="30" r="39" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="4" t="s">
-        <v>502</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>336</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>337</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>338</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>340</v>
-      </c>
-      <c r="G39" s="6" t="s">
-        <v>341</v>
-      </c>
-      <c r="H39" s="6" t="s">
-        <v>342</v>
-      </c>
-      <c r="I39" s="5" t="s">
-        <v>343</v>
-      </c>
-      <c r="J39" s="8" t="s">
-        <v>335</v>
-      </c>
-      <c r="K39" s="9">
-        <v>61468</v>
-      </c>
-      <c r="L39" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="30" r="40" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="7" t="s">
-        <v>503</v>
-      </c>
-      <c r="B40" s="5"/>
-      <c r="C40" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>346</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>347</v>
-      </c>
-      <c r="F40" s="6" t="s">
-        <v>348</v>
-      </c>
-      <c r="G40" s="6" t="s">
-        <v>349</v>
-      </c>
-      <c r="H40" s="6" t="s">
-        <v>350</v>
-      </c>
-      <c r="I40" s="5" t="s">
-        <v>351</v>
-      </c>
-      <c r="J40" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="K40" s="9">
-        <v>20223</v>
-      </c>
-      <c r="L40" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="30" r="41" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="4" t="s">
-        <v>504</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>352</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>353</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>354</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>355</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>356</v>
-      </c>
-      <c r="G41" s="6" t="s">
-        <v>357</v>
-      </c>
-      <c r="H41" s="6" t="s">
-        <v>358</v>
-      </c>
-      <c r="I41" s="5" t="s">
-        <v>359</v>
-      </c>
-      <c r="J41" s="8" t="s">
-        <v>300</v>
-      </c>
-      <c r="K41" s="9">
-        <v>48636</v>
-      </c>
-      <c r="L41" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="30" r="42" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="4" t="s">
-        <v>505</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>360</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>361</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>362</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>363</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>364</v>
-      </c>
-      <c r="G42" s="6" t="s">
-        <v>365</v>
-      </c>
-      <c r="H42" s="6" t="s">
-        <v>366</v>
-      </c>
-      <c r="I42" s="5" t="s">
-        <v>367</v>
-      </c>
-      <c r="J42" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="K42" s="9">
-        <v>30140</v>
-      </c>
-      <c r="L42" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="30" r="43" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="7" t="s">
-        <v>506</v>
-      </c>
-      <c r="B43" s="5"/>
-      <c r="C43" s="6" t="s">
-        <v>369</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>370</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>371</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>372</v>
-      </c>
-      <c r="G43" s="6" t="s">
-        <v>373</v>
-      </c>
-      <c r="H43" s="6" t="s">
-        <v>374</v>
-      </c>
-      <c r="I43" s="5" t="s">
-        <v>375</v>
-      </c>
-      <c r="J43" s="8" t="s">
-        <v>376</v>
-      </c>
-      <c r="K43" s="9">
-        <v>85381</v>
-      </c>
-      <c r="L43" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="30" r="44" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="4" t="s">
-        <v>507</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>377</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>378</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>379</v>
-      </c>
-      <c r="E44" s="10" t="s">
-        <v>380</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>381</v>
-      </c>
-      <c r="G44" s="6" t="s">
-        <v>382</v>
-      </c>
-      <c r="H44" s="6" t="s">
-        <v>383</v>
-      </c>
-      <c r="I44" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="J44" s="8" t="s">
-        <v>385</v>
-      </c>
-      <c r="K44" s="9">
-        <v>57073</v>
-      </c>
-      <c r="L44" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="30" r="45" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="4" t="s">
-        <v>508</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>386</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>387</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>388</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>389</v>
-      </c>
-      <c r="F45" s="6" t="s">
-        <v>390</v>
-      </c>
-      <c r="G45" s="6" t="s">
-        <v>391</v>
-      </c>
-      <c r="H45" s="6" t="s">
-        <v>392</v>
-      </c>
-      <c r="I45" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J45" s="8" t="s">
-        <v>393</v>
-      </c>
-      <c r="K45" s="9">
-        <v>65612</v>
-      </c>
-      <c r="L45" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="30" r="46" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="7" t="s">
-        <v>509</v>
-      </c>
-      <c r="B46" s="5"/>
-      <c r="C46" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>396</v>
-      </c>
-      <c r="E46" s="7" t="s">
-        <v>397</v>
-      </c>
-      <c r="F46" s="6" t="s">
-        <v>398</v>
-      </c>
-      <c r="G46" s="6" t="s">
-        <v>399</v>
-      </c>
-      <c r="H46" s="6" t="s">
-        <v>400</v>
-      </c>
-      <c r="I46" s="5" t="s">
-        <v>401</v>
-      </c>
-      <c r="J46" s="8" t="s">
-        <v>242</v>
-      </c>
-      <c r="K46" s="9">
-        <v>67448</v>
-      </c>
-      <c r="L46" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="30" r="47" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="4" t="s">
-        <v>510</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>402</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>403</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>404</v>
-      </c>
-      <c r="E47" s="7" t="s">
-        <v>405</v>
-      </c>
-      <c r="F47" s="6" t="s">
-        <v>406</v>
-      </c>
-      <c r="G47" s="6" t="s">
-        <v>407</v>
-      </c>
-      <c r="H47" s="6" t="s">
-        <v>408</v>
-      </c>
-      <c r="I47" s="5" t="s">
-        <v>409</v>
-      </c>
-      <c r="J47" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="K47" s="9">
-        <v>59405</v>
-      </c>
-      <c r="L47" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="29.25" r="48" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="4" t="s">
-        <v>511</v>
-      </c>
-      <c r="B48" s="5"/>
-      <c r="C48" s="6" t="s">
-        <v>411</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>412</v>
-      </c>
-      <c r="E48" s="7" t="s">
-        <v>413</v>
-      </c>
-      <c r="F48" s="6" t="s">
-        <v>414</v>
-      </c>
-      <c r="G48" s="6" t="s">
-        <v>415</v>
-      </c>
-      <c r="H48" s="6" t="s">
-        <v>416</v>
-      </c>
-      <c r="I48" s="5" t="s">
-        <v>417</v>
-      </c>
-      <c r="J48" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="K48" s="9">
-        <v>92563</v>
-      </c>
-      <c r="L48" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="30" r="49" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="7" t="s">
-        <v>512</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>418</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>419</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>420</v>
-      </c>
-      <c r="E49" s="7" t="s">
-        <v>421</v>
-      </c>
-      <c r="F49" s="6" t="s">
-        <v>422</v>
-      </c>
-      <c r="G49" s="6" t="s">
-        <v>423</v>
-      </c>
-      <c r="H49" s="6" t="s">
-        <v>424</v>
-      </c>
-      <c r="I49" s="5" t="s">
-        <v>425</v>
-      </c>
-      <c r="J49" s="8" t="s">
-        <v>426</v>
-      </c>
-      <c r="K49" s="9">
-        <v>94271</v>
-      </c>
-      <c r="L49" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="30" r="50" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="4" t="s">
-        <v>513</v>
-      </c>
-      <c r="B50" s="5"/>
-      <c r="C50" s="6" t="s">
-        <v>428</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>429</v>
-      </c>
-      <c r="E50" s="7" t="s">
-        <v>430</v>
-      </c>
-      <c r="F50" s="6" t="s">
-        <v>431</v>
-      </c>
-      <c r="G50" s="6" t="s">
-        <v>432</v>
-      </c>
-      <c r="H50" s="6" t="s">
-        <v>433</v>
-      </c>
-      <c r="I50" s="5" t="s">
-        <v>434</v>
-      </c>
-      <c r="J50" s="8" t="s">
-        <v>435</v>
-      </c>
-      <c r="K50" s="9">
-        <v>77230</v>
-      </c>
-      <c r="L50" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row ht="30" r="51" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="4" t="s">
-        <v>514</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>436</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>437</v>
-      </c>
-      <c r="D51" s="6" t="s">
-        <v>438</v>
-      </c>
-      <c r="E51" s="7" t="s">
-        <v>439</v>
-      </c>
-      <c r="F51" s="6" t="s">
-        <v>440</v>
-      </c>
-      <c r="G51" s="6" t="s">
-        <v>441</v>
-      </c>
-      <c r="H51" s="6" t="s">
-        <v>442</v>
-      </c>
-      <c r="I51" s="5" t="s">
-        <v>443</v>
-      </c>
-      <c r="J51" s="8" t="s">
-        <v>444</v>
-      </c>
-      <c r="K51" s="9">
-        <v>34712</v>
-      </c>
-      <c r="L51" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Tests for different browsers
</commit_message>
<xml_diff>
--- a/FinalProject/data/pet-store-data.xlsx
+++ b/FinalProject/data/pet-store-data.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21225" windowHeight="6720" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="cart_items" sheetId="1" r:id="rId1"/>
     <sheet name="users" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1:J12"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -1416,8 +1415,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1584,14 +1583,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1638,7 +1629,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1670,10 +1661,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1705,7 +1695,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1881,20 +1870,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28.140625" customWidth="1"/>
     <col min="2" max="2" width="108" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1902,7 +1891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="12" t="s">
         <v>445</v>
       </c>
@@ -1910,7 +1899,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="12" t="s">
         <v>447</v>
       </c>
@@ -1918,7 +1907,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="12" t="s">
         <v>449</v>
       </c>
@@ -1926,7 +1915,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="12" t="s">
         <v>452</v>
       </c>
@@ -1934,7 +1923,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="12" t="s">
         <v>454</v>
       </c>
@@ -1942,7 +1931,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" s="12" t="s">
         <v>455</v>
       </c>
@@ -1950,7 +1939,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" s="12" t="s">
         <v>458</v>
       </c>
@@ -1958,7 +1947,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" s="12" t="s">
         <v>460</v>
       </c>
@@ -1966,7 +1955,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10" s="12" t="s">
         <v>462</v>
       </c>
@@ -1974,7 +1963,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" s="12" t="s">
         <v>463</v>
       </c>
@@ -2000,14 +1989,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="4" width="17.28515625" style="3"/>
     <col min="5" max="5" width="25.85546875" style="3" customWidth="1"/>
@@ -2016,7 +2005,7 @@
     <col min="8" max="16384" width="17.28515625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="30.75" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2054,7 +2043,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="44.25" thickBot="1">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -2092,7 +2081,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="44.25" thickBot="1">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -2130,7 +2119,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="58.5" thickBot="1">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -2168,7 +2157,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="58.5" thickBot="1">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -2206,7 +2195,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="44.25" thickBot="1">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -2244,7 +2233,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="44.25" thickBot="1">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -2282,7 +2271,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="44.25" thickBot="1">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -2320,7 +2309,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="44.25" thickBot="1">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -2358,7 +2347,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="58.5" thickBot="1">
       <c r="A10" s="7">
         <v>9</v>
       </c>
@@ -2396,7 +2385,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="58.5" thickBot="1">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -2434,7 +2423,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="58.5" thickBot="1">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -2472,7 +2461,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="44.25" thickBot="1">
       <c r="A13" s="7">
         <v>12</v>
       </c>
@@ -2510,7 +2499,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="44.25" thickBot="1">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -2548,7 +2537,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="44.25" thickBot="1">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -2586,7 +2575,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="44.25" thickBot="1">
       <c r="A16" s="7">
         <v>15</v>
       </c>
@@ -2624,7 +2613,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="44.25" thickBot="1">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -2662,7 +2651,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="44.25" thickBot="1">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -2700,7 +2689,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="44.25" thickBot="1">
       <c r="A19" s="7">
         <v>18</v>
       </c>
@@ -2738,7 +2727,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="44.25" thickBot="1">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -2776,7 +2765,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="44.25" thickBot="1">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -2814,7 +2803,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" ht="44.25" thickBot="1">
       <c r="A22" s="7">
         <v>21</v>
       </c>
@@ -2852,7 +2841,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" ht="58.5" thickBot="1">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -2890,7 +2879,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" ht="44.25" thickBot="1">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -2928,7 +2917,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" ht="58.5" thickBot="1">
       <c r="A25" s="7">
         <v>24</v>
       </c>
@@ -2966,7 +2955,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" ht="58.5" thickBot="1">
       <c r="A26" s="4">
         <v>25</v>
       </c>
@@ -3004,7 +2993,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" ht="58.5" thickBot="1">
       <c r="A27" s="4">
         <v>26</v>
       </c>
@@ -3042,7 +3031,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" ht="44.25" thickBot="1">
       <c r="A28" s="7">
         <v>27</v>
       </c>
@@ -3080,7 +3069,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" ht="58.5" thickBot="1">
       <c r="A29" s="4">
         <v>28</v>
       </c>
@@ -3118,7 +3107,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" ht="44.25" thickBot="1">
       <c r="A30" s="4">
         <v>29</v>
       </c>
@@ -3156,7 +3145,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" ht="58.5" thickBot="1">
       <c r="A31" s="7">
         <v>30</v>
       </c>
@@ -3194,7 +3183,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" ht="44.25" thickBot="1">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -3232,7 +3221,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" ht="58.5" thickBot="1">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -3270,7 +3259,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" ht="44.25" thickBot="1">
       <c r="A34" s="7">
         <v>33</v>
       </c>
@@ -3308,7 +3297,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" ht="58.5" thickBot="1">
       <c r="A35" s="4">
         <v>34</v>
       </c>
@@ -3346,7 +3335,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" ht="58.5" thickBot="1">
       <c r="A36" s="4">
         <v>35</v>
       </c>
@@ -3384,7 +3373,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" ht="44.25" thickBot="1">
       <c r="A37" s="7">
         <v>36</v>
       </c>
@@ -3422,7 +3411,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" ht="44.25" thickBot="1">
       <c r="A38" s="4">
         <v>37</v>
       </c>
@@ -3460,7 +3449,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" ht="58.5" thickBot="1">
       <c r="A39" s="4">
         <v>38</v>
       </c>
@@ -3498,7 +3487,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" ht="44.25" thickBot="1">
       <c r="A40" s="7">
         <v>39</v>
       </c>
@@ -3536,7 +3525,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" ht="44.25" thickBot="1">
       <c r="A41" s="4">
         <v>40</v>
       </c>
@@ -3574,7 +3563,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" ht="58.5" thickBot="1">
       <c r="A42" s="4">
         <v>41</v>
       </c>
@@ -3612,7 +3601,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" ht="44.25" thickBot="1">
       <c r="A43" s="7">
         <v>42</v>
       </c>
@@ -3650,7 +3639,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" ht="58.5" thickBot="1">
       <c r="A44" s="4">
         <v>43</v>
       </c>
@@ -3688,7 +3677,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" ht="58.5" thickBot="1">
       <c r="A45" s="4">
         <v>44</v>
       </c>
@@ -3726,7 +3715,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" ht="44.25" thickBot="1">
       <c r="A46" s="7">
         <v>45</v>
       </c>
@@ -3764,7 +3753,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" ht="58.5" thickBot="1">
       <c r="A47" s="4">
         <v>46</v>
       </c>
@@ -3802,7 +3791,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" ht="44.25" thickBot="1">
       <c r="A48" s="4">
         <v>47</v>
       </c>
@@ -3840,7 +3829,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" ht="44.25" thickBot="1">
       <c r="A49" s="7">
         <v>48</v>
       </c>
@@ -3878,7 +3867,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" ht="44.25" thickBot="1">
       <c r="A50" s="4">
         <v>49</v>
       </c>
@@ -3916,7 +3905,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" ht="44.25" thickBot="1">
       <c r="A51" s="4">
         <v>50</v>
       </c>

</xml_diff>